<commit_message>
Use slugs for all
</commit_message>
<xml_diff>
--- a/peliculas.xlsx
+++ b/peliculas.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="91">
   <si>
     <t>title</t>
   </si>
@@ -255,6 +255,49 @@
   </si>
   <si>
     <t>https://www.youtube.com/embed/lkCzphE86-4</t>
+  </si>
+  <si>
+    <t>Star Spangled to Death</t>
+  </si>
+  <si>
+    <t>Ken Jacobs</t>
+  </si>
+  <si>
+    <t>Documentary, History</t>
+  </si>
+  <si>
+    <t>Jack Smith, Jerry Sims, Gib Taylor</t>
+  </si>
+  <si>
+    <t>https://images-na.ssl-images-amazon.com/images/M/MV5BMDFkYmQ5MjMtZjY5ZS00MWFjLTlkM2MtODk1YmQ0ZDFhOTNlXkEyXkFqcGdeQXVyMjYxMzY2NDk@._V1_UY268_CR103,0,182,268_AL_.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">An examination of the history of the U.S. through archival footage and contrasting views of society.
+</t>
+  </si>
+  <si>
+    <t>Los Angeles Film Critics Association Awards - Independent/Experimental Film and Video Award</t>
+  </si>
+  <si>
+    <t>The Law of Sodom</t>
+  </si>
+  <si>
+    <t>James Quinn</t>
+  </si>
+  <si>
+    <t>Short, Drama, Horror</t>
+  </si>
+  <si>
+    <t>James Quinn, Carol Lieb</t>
+  </si>
+  <si>
+    <t>https://images-na.ssl-images-amazon.com/images/M/MV5BOWEzMjU5MzYtNDUzOS00NWUzLWEyNTAtOWVkMmMyNzQ5MDRiXkEyXkFqcGdeQXVyNjY4NzU5MDE@._V1_UY268_CR43,0,182,268_AL_.jpg</t>
+  </si>
+  <si>
+    <t>Austria</t>
+  </si>
+  <si>
+    <t>The Law of Sodom tells the psychedelic story of a paranoid schizophrenic, all through grotesque imagery, surreal worlds, intense atmosphere and violent eruptions, written, directed and shot by a schizophrenic completely while being psychotic, giving the film a very unique feeling.</t>
   </si>
 </sst>
 </file>
@@ -622,23 +665,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="32.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="50.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="51.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="34.7109375" style="1" customWidth="1"/>
     <col min="10" max="10" width="37.42578125" customWidth="1"/>
+    <col min="11" max="11" width="86.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -670,7 +717,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -702,7 +749,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>50</v>
       </c>
@@ -734,7 +781,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -766,7 +813,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -798,7 +845,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="120" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>36</v>
       </c>
@@ -830,7 +877,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>49</v>
       </c>
@@ -862,7 +909,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="105" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>58</v>
       </c>
@@ -894,7 +941,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>63</v>
       </c>
@@ -926,7 +973,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>70</v>
       </c>
@@ -956,6 +1003,61 @@
       </c>
       <c r="J10" s="1" t="s">
         <v>73</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>77</v>
+      </c>
+      <c r="B11">
+        <v>2004</v>
+      </c>
+      <c r="C11" t="s">
+        <v>78</v>
+      </c>
+      <c r="E11" t="s">
+        <v>79</v>
+      </c>
+      <c r="F11" t="s">
+        <v>80</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="I11" t="s">
+        <v>14</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="K11" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="120" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>84</v>
+      </c>
+      <c r="B12">
+        <v>2016</v>
+      </c>
+      <c r="C12" t="s">
+        <v>85</v>
+      </c>
+      <c r="E12" t="s">
+        <v>86</v>
+      </c>
+      <c r="F12" t="s">
+        <v>87</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="I12" t="s">
+        <v>89</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -978,8 +1080,10 @@
     <hyperlink ref="G9" r:id="rId16"/>
     <hyperlink ref="H10" r:id="rId17"/>
     <hyperlink ref="G10" r:id="rId18"/>
+    <hyperlink ref="H11" r:id="rId19"/>
+    <hyperlink ref="H12" r:id="rId20"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId19"/>
+  <pageSetup orientation="portrait" r:id="rId21"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added user login, register, logout and carousel
</commit_message>
<xml_diff>
--- a/peliculas.xlsx
+++ b/peliculas.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="peliculas" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="116">
   <si>
     <t>title</t>
   </si>
@@ -272,10 +272,6 @@
     <t>https://images-na.ssl-images-amazon.com/images/M/MV5BMDFkYmQ5MjMtZjY5ZS00MWFjLTlkM2MtODk1YmQ0ZDFhOTNlXkEyXkFqcGdeQXVyMjYxMzY2NDk@._V1_UY268_CR103,0,182,268_AL_.jpg</t>
   </si>
   <si>
-    <t xml:space="preserve">An examination of the history of the U.S. through archival footage and contrasting views of society.
-</t>
-  </si>
-  <si>
     <t>Los Angeles Film Critics Association Awards - Independent/Experimental Film and Video Award</t>
   </si>
   <si>
@@ -298,13 +294,91 @@
   </si>
   <si>
     <t>The Law of Sodom tells the psychedelic story of a paranoid schizophrenic, all through grotesque imagery, surreal worlds, intense atmosphere and violent eruptions, written, directed and shot by a schizophrenic completely while being psychotic, giving the film a very unique feeling.</t>
+  </si>
+  <si>
+    <t>Duel</t>
+  </si>
+  <si>
+    <t>https://player.vimeo.com/video/121321455</t>
+  </si>
+  <si>
+    <t>https://player.vimeo.com/video/169757501</t>
+  </si>
+  <si>
+    <t>https://images-na.ssl-images-amazon.com/images/M/MV5BZjkwYjY3OTYtMjA1NC00OGY0LTgzNTItNjFmMmMwZGYwNjkyXkEyXkFqcGdeQXVyMTQxNzMzNDI@._V1_UX182_CR0,0,182,268_AL_.jpg</t>
+  </si>
+  <si>
+    <t>Steven Spielberg</t>
+  </si>
+  <si>
+    <t>Action, Thriller</t>
+  </si>
+  <si>
+    <t>Dennis Weaver, Jacqueline Scott, Eddie Firestone</t>
+  </si>
+  <si>
+    <t>Primetime Emmy Awards - Primetime Emmy | Avoriaz Fantastic Film Festival - Grand Prize | Taormina International Film Festival - Best First Film</t>
+  </si>
+  <si>
+    <t>A business commuter is pursued and terrorized by the malevolent driver of a massive tractor-trailer.</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/5MtAMc4i8OA</t>
+  </si>
+  <si>
+    <t>Blindfold</t>
+  </si>
+  <si>
+    <t>Philip Dunne</t>
+  </si>
+  <si>
+    <t>Rock Hudson, Claudia Cardinale, Jack Warden</t>
+  </si>
+  <si>
+    <t>Comedy, Crime, Mystery</t>
+  </si>
+  <si>
+    <t>https://images-na.ssl-images-amazon.com/images/M/MV5BNmNiODUwYmMtNDNjMi00MDE2LWJjMjYtZTY1MzU5NjUwZTQ4XkEyXkFqcGdeQXVyNTgwNTk5MDU@._V1_UY268_CR0,0,182,268_AL_.jpg</t>
+  </si>
+  <si>
+    <t>A New York psychiatrist is solicited by government agents in connection with a former patient of his who also happens to be a scientist wanted by certain foreign powers.</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/iyXFPUrWjIA</t>
+  </si>
+  <si>
+    <t>https://images-na.ssl-images-amazon.com/images/M/MV5BMTA0Y2UyMDUtZGZiOS00ZmVkLTg3NmItODQyNTY1ZjU1MWE4L2ltYWdlL2ltYWdlXkEyXkFqcGdeQXVyNjc1NTYyMjg@._V1_UX182_CR0,0,182,268_AL_.jpg</t>
+  </si>
+  <si>
+    <t>Comedy, Mystery, Romance</t>
+  </si>
+  <si>
+    <t>Romance and suspense ensue in Paris as a woman is pursued by several men who want a fortune her murdered husband had stolen. Who can she trust?</t>
+  </si>
+  <si>
+    <t>Stanley Donen</t>
+  </si>
+  <si>
+    <t>Cary Grant, Audrey Hepburn, Walter Matthau</t>
+  </si>
+  <si>
+    <t>Charade</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/V7s0H9Qz168</t>
+  </si>
+  <si>
+    <t>BAFTA Awards - BAFTA Film Award | David di Donatello Awards - Golden Plate | Edgar Allan Poe Awards - Edgar</t>
+  </si>
+  <si>
+    <t>An examination of the history of the U.S. through archival footage and contrasting views of society.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -316,6 +390,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -342,12 +424,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -665,10 +751,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1015,12 +1101,18 @@
       <c r="C11" t="s">
         <v>78</v>
       </c>
+      <c r="D11">
+        <v>13</v>
+      </c>
       <c r="E11" t="s">
         <v>79</v>
       </c>
       <c r="F11" t="s">
         <v>80</v>
       </c>
+      <c r="G11" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="H11" s="2" t="s">
         <v>81</v>
       </c>
@@ -1028,37 +1120,148 @@
         <v>14</v>
       </c>
       <c r="J11" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="K11" t="s">
         <v>82</v>
-      </c>
-      <c r="K11" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B12">
         <v>2016</v>
       </c>
       <c r="C12" t="s">
+        <v>84</v>
+      </c>
+      <c r="D12">
+        <v>13</v>
+      </c>
+      <c r="E12" t="s">
         <v>85</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>86</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="H12" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="I12" t="s">
         <v>88</v>
       </c>
-      <c r="I12" t="s">
+      <c r="J12" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="J12" s="1" t="s">
+    </row>
+    <row r="13" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>90</v>
       </c>
+      <c r="B13">
+        <v>1971</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D13">
+        <v>13</v>
+      </c>
+      <c r="E13" t="s">
+        <v>95</v>
+      </c>
+      <c r="F13" t="s">
+        <v>96</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="I13" t="s">
+        <v>14</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="K13" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>100</v>
+      </c>
+      <c r="B14">
+        <v>1965</v>
+      </c>
+      <c r="C14" t="s">
+        <v>101</v>
+      </c>
+      <c r="D14">
+        <v>13</v>
+      </c>
+      <c r="E14" t="s">
+        <v>103</v>
+      </c>
+      <c r="F14" t="s">
+        <v>102</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="I14" t="s">
+        <v>14</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>112</v>
+      </c>
+      <c r="B15">
+        <v>1963</v>
+      </c>
+      <c r="C15" t="s">
+        <v>110</v>
+      </c>
+      <c r="D15">
+        <v>13</v>
+      </c>
+      <c r="E15" t="s">
+        <v>108</v>
+      </c>
+      <c r="F15" t="s">
+        <v>111</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="I15" t="s">
+        <v>14</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="K15" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D16" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1082,8 +1285,16 @@
     <hyperlink ref="G10" r:id="rId18"/>
     <hyperlink ref="H11" r:id="rId19"/>
     <hyperlink ref="H12" r:id="rId20"/>
+    <hyperlink ref="G11" r:id="rId21"/>
+    <hyperlink ref="G12" r:id="rId22"/>
+    <hyperlink ref="H13" r:id="rId23"/>
+    <hyperlink ref="G13" r:id="rId24"/>
+    <hyperlink ref="H14" r:id="rId25"/>
+    <hyperlink ref="G14" r:id="rId26"/>
+    <hyperlink ref="H15" r:id="rId27"/>
+    <hyperlink ref="G15" r:id="rId28"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId21"/>
+  <pageSetup orientation="portrait" r:id="rId29"/>
 </worksheet>
 </file>
</xml_diff>